<commit_message>
Mon Aug 20 14:43:23 EDT 2018
</commit_message>
<xml_diff>
--- a/WoFM RPG/Assets/JS/map.xlsx
+++ b/WoFM RPG/Assets/JS/map.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\588648\Unity\WoFM RPG\Assets\JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FC13F73C-6B08-4075-A883-0DFB0BE07DBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7872"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -506,11 +507,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="XG1330:YF1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="XK1323" workbookViewId="0">
-      <selection activeCell="XR1341" sqref="XR1341"/>
+    <sheetView tabSelected="1" topLeftCell="XM1323" workbookViewId="0">
+      <selection activeCell="YA1342" sqref="YA1342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fri Sep 21 23:38:17 EDT 2018
</commit_message>
<xml_diff>
--- a/WoFM RPG/Assets/JS/map.xlsx
+++ b/WoFM RPG/Assets/JS/map.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\588648\Unity\WoFM RPG\Assets\JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FC13F73C-6B08-4075-A883-0DFB0BE07DBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FD19AB62-1213-4801-B5F1-B3B503587E66}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,24 +25,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ROOM 1</t>
-  </si>
-  <si>
-    <t>ROOM 12</t>
-  </si>
-  <si>
-    <t>ROOM 139</t>
   </si>
   <si>
     <t>ROOM 71</t>
   </si>
   <si>
-    <t>ROOM 43</t>
+    <t>ROOM 82</t>
   </si>
   <si>
-    <t>ROOM 82</t>
+    <t>ROOM 343</t>
+  </si>
+  <si>
+    <t>ROOM 301</t>
+  </si>
+  <si>
+    <t>ROOM 208</t>
+  </si>
+  <si>
+    <t>ROOM 397</t>
+  </si>
+  <si>
+    <t>ROOM 363</t>
+  </si>
+  <si>
+    <t>ROOM 370</t>
+  </si>
+  <si>
+    <t>ROOM 42</t>
+  </si>
+  <si>
+    <t>ROOM 113</t>
+  </si>
+  <si>
+    <t>ROOM 257</t>
+  </si>
+  <si>
+    <t>ROOM 168</t>
+  </si>
+  <si>
+    <t>ROOM 78</t>
+  </si>
+  <si>
+    <t>ROOM 159</t>
+  </si>
+  <si>
+    <t>ROOM 278</t>
+  </si>
+  <si>
+    <t>ROOM 285</t>
+  </si>
+  <si>
+    <t>ROOM 36</t>
+  </si>
+  <si>
+    <t>ROOM 314</t>
+  </si>
+  <si>
+    <t>ROOM 155</t>
   </si>
 </sst>
 </file>
@@ -508,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="XG1330:YF1341"/>
+  <dimension ref="XA1306:YF1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="XM1323" workbookViewId="0">
-      <selection activeCell="YA1342" sqref="YA1342"/>
+    <sheetView tabSelected="1" topLeftCell="XG1328" workbookViewId="0">
+      <selection activeCell="XU1310" sqref="XU1310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,632 +571,1804 @@
     <col min="1262" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1330" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1306" spans="640:646" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1307" spans="640:646" x14ac:dyDescent="0.3">
+      <c r="XP1307" s="7" t="str">
+        <f t="shared" ref="XP1307:XV1311" ca="1" si="0">CONCATENATE(CELL("col",XP1307)-1,",",CELL("row",XP1307)-1)</f>
+        <v>639,1306</v>
+      </c>
+      <c r="XQ1307" s="16">
+        <v>300</v>
+      </c>
+      <c r="XR1307" s="9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>641,1306</v>
+      </c>
+      <c r="XS1307" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>642,1306</v>
+      </c>
+      <c r="XT1307" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>643,1306</v>
+      </c>
+      <c r="XU1307" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>644,1306</v>
+      </c>
+      <c r="XV1307" s="9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>645,1306</v>
+      </c>
+    </row>
+    <row r="1308" spans="640:646" x14ac:dyDescent="0.3">
+      <c r="XP1308" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>639,1307</v>
+      </c>
+      <c r="XQ1308" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>640,1307</v>
+      </c>
+      <c r="XR1308" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>641,1307</v>
+      </c>
+      <c r="XS1308" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>642,1307</v>
+      </c>
+      <c r="XT1308" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>643,1307</v>
+      </c>
+      <c r="XU1308" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>644,1307</v>
+      </c>
+      <c r="XV1308" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>645,1307</v>
+      </c>
+    </row>
+    <row r="1309" spans="640:646" x14ac:dyDescent="0.3">
+      <c r="XP1309" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>639,1308</v>
+      </c>
+      <c r="XQ1309" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="XR1309" s="4">
+        <v>223</v>
+      </c>
+      <c r="XS1309" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>642,1308</v>
+      </c>
+      <c r="XT1309" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>643,1308</v>
+      </c>
+      <c r="XU1309" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="XV1309" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>645,1308</v>
+      </c>
+    </row>
+    <row r="1310" spans="640:646" x14ac:dyDescent="0.3">
+      <c r="XP1310" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>639,1309</v>
+      </c>
+      <c r="XQ1310" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>640,1309</v>
+      </c>
+      <c r="XR1310" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>641,1309</v>
+      </c>
+      <c r="XS1310" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>642,1309</v>
+      </c>
+      <c r="XT1310" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>643,1309</v>
+      </c>
+      <c r="XU1310" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>644,1309</v>
+      </c>
+      <c r="XV1310" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>645,1309</v>
+      </c>
+    </row>
+    <row r="1311" spans="640:646" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XP1311" s="11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>639,1310</v>
+      </c>
+      <c r="XQ1311" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>640,1310</v>
+      </c>
+      <c r="XR1311" s="15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>641,1310</v>
+      </c>
+      <c r="XS1311" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>642,1310</v>
+      </c>
+      <c r="XT1311" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>643,1310</v>
+      </c>
+      <c r="XU1311" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>644,1310</v>
+      </c>
+      <c r="XV1311" s="15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>645,1310</v>
+      </c>
+    </row>
+    <row r="1312" spans="640:646" x14ac:dyDescent="0.3">
+      <c r="XP1312" s="7" t="str">
+        <f t="shared" ref="XP1312:XV1316" ca="1" si="1">CONCATENATE(CELL("col",XP1312)-1,",",CELL("row",XP1312)-1)</f>
+        <v>639,1311</v>
+      </c>
+      <c r="XQ1312" s="16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>640,1311</v>
+      </c>
+      <c r="XR1312" s="9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>641,1311</v>
+      </c>
+      <c r="XS1312" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>642,1311</v>
+      </c>
+      <c r="XT1312" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>643,1311</v>
+      </c>
+      <c r="XU1312" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>644,1311</v>
+      </c>
+      <c r="XV1312" s="9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>645,1311</v>
+      </c>
+    </row>
+    <row r="1313" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XP1313" s="10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>639,1312</v>
+      </c>
+      <c r="XQ1313" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>640,1312</v>
+      </c>
+      <c r="XR1313" s="14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>641,1312</v>
+      </c>
+      <c r="XS1313" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>642,1312</v>
+      </c>
+      <c r="XT1313" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>643,1312</v>
+      </c>
+      <c r="XU1313" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>644,1312</v>
+      </c>
+      <c r="XV1313" s="14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>645,1312</v>
+      </c>
+    </row>
+    <row r="1314" spans="625:652" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XP1314" s="10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>639,1313</v>
+      </c>
+      <c r="XQ1314" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="XR1314" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>641,1313</v>
+      </c>
+      <c r="XS1314" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>642,1313</v>
+      </c>
+      <c r="XT1314" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>643,1313</v>
+      </c>
+      <c r="XU1314" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="XV1314" s="14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>645,1313</v>
+      </c>
+    </row>
+    <row r="1315" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XA1315" s="7" t="str">
+        <f t="shared" ref="XA1315:XA1321" ca="1" si="2">CONCATENATE(CELL("col",XA1315)-1,",",CELL("row",XA1315)-1)</f>
+        <v>624,1314</v>
+      </c>
+      <c r="XB1315" s="8" t="str">
+        <f t="shared" ref="XA1315:XF1320" ca="1" si="3">CONCATENATE(CELL("col",XB1315)-1,",",CELL("row",XB1315)-1)</f>
+        <v>625,1314</v>
+      </c>
+      <c r="XC1315" s="8" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>626,1314</v>
+      </c>
+      <c r="XD1315" s="8" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>627,1314</v>
+      </c>
+      <c r="XE1315" s="8" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>628,1314</v>
+      </c>
+      <c r="XF1315" s="9" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>629,1314</v>
+      </c>
+      <c r="XP1315" s="10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>639,1314</v>
+      </c>
+      <c r="XQ1315" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>640,1314</v>
+      </c>
+      <c r="XR1315" s="14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>641,1314</v>
+      </c>
+      <c r="XS1315" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>642,1314</v>
+      </c>
+      <c r="XT1315" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>643,1314</v>
+      </c>
+      <c r="XU1315" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>644,1314</v>
+      </c>
+      <c r="XV1315" s="14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>645,1314</v>
+      </c>
+      <c r="XW1315" s="7" t="str">
+        <f t="shared" ref="XW1315:YB1321" ca="1" si="4">CONCATENATE(CELL("col",XW1315)-1,",",CELL("row",XW1315)-1)</f>
+        <v>646,1314</v>
+      </c>
+      <c r="XX1315" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>647,1314</v>
+      </c>
+      <c r="XY1315" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>648,1314</v>
+      </c>
+      <c r="XZ1315" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>649,1314</v>
+      </c>
+      <c r="YA1315" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>650,1314</v>
+      </c>
+      <c r="YB1315" s="9" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>651,1314</v>
+      </c>
+    </row>
+    <row r="1316" spans="625:652" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XA1316" s="10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>624,1315</v>
+      </c>
+      <c r="XB1316" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>625,1315</v>
+      </c>
+      <c r="XC1316" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>626,1315</v>
+      </c>
+      <c r="XD1316" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>627,1315</v>
+      </c>
+      <c r="XE1316" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>628,1315</v>
+      </c>
+      <c r="XF1316" s="14" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>629,1315</v>
+      </c>
+      <c r="XP1316" s="11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>639,1315</v>
+      </c>
+      <c r="XQ1316" s="5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>640,1315</v>
+      </c>
+      <c r="XR1316" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>641,1315</v>
+      </c>
+      <c r="XS1316" s="13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>642,1315</v>
+      </c>
+      <c r="XT1316" s="13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>643,1315</v>
+      </c>
+      <c r="XU1316" s="13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>644,1315</v>
+      </c>
+      <c r="XV1316" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>645,1315</v>
+      </c>
+      <c r="XW1316" s="10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>646,1315</v>
+      </c>
+      <c r="XX1316" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>647,1315</v>
+      </c>
+      <c r="XY1316" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>648,1315</v>
+      </c>
+      <c r="XZ1316" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>649,1315</v>
+      </c>
+      <c r="YA1316" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>650,1315</v>
+      </c>
+      <c r="YB1316" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>651,1315</v>
+      </c>
+    </row>
+    <row r="1317" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XA1317" s="10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>624,1316</v>
+      </c>
+      <c r="XB1317" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>625,1316</v>
+      </c>
+      <c r="XC1317" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>626,1316</v>
+      </c>
+      <c r="XD1317" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>627,1316</v>
+      </c>
+      <c r="XE1317" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>628,1316</v>
+      </c>
+      <c r="XF1317" s="14" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>629,1316</v>
+      </c>
+      <c r="XG1317" s="7" t="str">
+        <f t="shared" ref="XG1317:XK1319" ca="1" si="5">CONCATENATE(CELL("col",XG1317)-1,",",CELL("row",XG1317)-1)</f>
+        <v>630,1316</v>
+      </c>
+      <c r="XH1317" s="8" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>631,1316</v>
+      </c>
+      <c r="XI1317" s="8" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>632,1316</v>
+      </c>
+      <c r="XJ1317" s="8" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>633,1316</v>
+      </c>
+      <c r="XK1317" s="8" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>634,1316</v>
+      </c>
+      <c r="XL1317" s="7" t="str">
+        <f t="shared" ref="XL1316:XW1319" ca="1" si="6">CONCATENATE(CELL("col",XL1317)-1,",",CELL("row",XL1317)-1)</f>
+        <v>635,1316</v>
+      </c>
+      <c r="XM1317" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>636,1316</v>
+      </c>
+      <c r="XN1317" s="9" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>637,1316</v>
+      </c>
+      <c r="XO1317" s="7" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>638,1316</v>
+      </c>
+      <c r="XP1317" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>639,1316</v>
+      </c>
+      <c r="XQ1317" s="16" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>640,1316</v>
+      </c>
+      <c r="XR1317" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>641,1316</v>
+      </c>
+      <c r="XS1317" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>642,1316</v>
+      </c>
+      <c r="XT1317" s="7" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>643,1316</v>
+      </c>
+      <c r="XU1317" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>644,1316</v>
+      </c>
+      <c r="XV1317" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>645,1316</v>
+      </c>
+      <c r="XW1317" s="10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>646,1316</v>
+      </c>
+      <c r="XX1317" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>647,1316</v>
+      </c>
+      <c r="XY1317" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>648,1316</v>
+      </c>
+      <c r="XZ1317" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>649,1316</v>
+      </c>
+      <c r="YA1317" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>650,1316</v>
+      </c>
+      <c r="YB1317" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>651,1316</v>
+      </c>
+    </row>
+    <row r="1318" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XA1318" s="10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>624,1317</v>
+      </c>
+      <c r="XB1318" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>625,1317</v>
+      </c>
+      <c r="XC1318" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="XD1318" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>627,1317</v>
+      </c>
+      <c r="XE1318" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>628,1317</v>
+      </c>
+      <c r="XF1318" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>629,1317</v>
+      </c>
+      <c r="XG1318" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>630,1317</v>
+      </c>
+      <c r="XH1318" s="3" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>631,1317</v>
+      </c>
+      <c r="XI1318" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="XJ1318" s="3" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>633,1317</v>
+      </c>
+      <c r="XK1318" s="3" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>634,1317</v>
+      </c>
+      <c r="XL1318" s="2" t="str">
+        <f t="shared" ref="XL1316:XS1320" ca="1" si="7">CONCATENATE(CELL("col",XL1318)-1,",",CELL("row",XL1318)-1)</f>
+        <v>635,1317</v>
+      </c>
+      <c r="XM1318" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="XN1318" s="4" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>637,1317</v>
+      </c>
+      <c r="XO1318" s="2" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>638,1317</v>
+      </c>
+      <c r="XP1318" s="3" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>639,1317</v>
+      </c>
+      <c r="XQ1318" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="XR1318" s="3" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>641,1317</v>
+      </c>
+      <c r="XS1318" s="3" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>642,1317</v>
+      </c>
+      <c r="XT1318" s="2" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>643,1317</v>
+      </c>
+      <c r="XU1318" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="XV1318" s="3" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>645,1317</v>
+      </c>
+      <c r="XW1318" s="2" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>646,1317</v>
+      </c>
+      <c r="XX1318" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>647,1317</v>
+      </c>
+      <c r="XY1318" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="XZ1318" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>649,1317</v>
+      </c>
+      <c r="YA1318" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>650,1317</v>
+      </c>
+      <c r="YB1318" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>651,1317</v>
+      </c>
+    </row>
+    <row r="1319" spans="625:652" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XA1319" s="10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>624,1318</v>
+      </c>
+      <c r="XB1319" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>625,1318</v>
+      </c>
+      <c r="XC1319" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>626,1318</v>
+      </c>
+      <c r="XD1319" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>627,1318</v>
+      </c>
+      <c r="XE1319" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>628,1318</v>
+      </c>
+      <c r="XF1319" s="14" t="str">
+        <f t="shared" ref="XF1319:XK1325" ca="1" si="8">CONCATENATE(CELL("col",XF1319)-1,",",CELL("row",XF1319)-1)</f>
+        <v>629,1318</v>
+      </c>
+      <c r="XG1319" s="11" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>630,1318</v>
+      </c>
+      <c r="XH1319" s="13" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>631,1318</v>
+      </c>
+      <c r="XI1319" s="13" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>632,1318</v>
+      </c>
+      <c r="XJ1319" s="13" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>633,1318</v>
+      </c>
+      <c r="XK1319" s="13" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>634,1318</v>
+      </c>
+      <c r="XL1319" s="10" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>635,1318</v>
+      </c>
+      <c r="XM1319" s="3" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>636,1318</v>
+      </c>
+      <c r="XN1319" s="14" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>637,1318</v>
+      </c>
+      <c r="XO1319" s="11" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>638,1318</v>
+      </c>
+      <c r="XP1319" s="13" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>639,1318</v>
+      </c>
+      <c r="XQ1319" s="13" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>640,1318</v>
+      </c>
+      <c r="XR1319" s="13" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>641,1318</v>
+      </c>
+      <c r="XS1319" s="13" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>642,1318</v>
+      </c>
+      <c r="XT1319" s="11" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>643,1318</v>
+      </c>
+      <c r="XU1319" s="13" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>644,1318</v>
+      </c>
+      <c r="XV1319" s="13" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>645,1318</v>
+      </c>
+      <c r="XW1319" s="10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>646,1318</v>
+      </c>
+      <c r="XX1319" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>647,1318</v>
+      </c>
+      <c r="XY1319" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>648,1318</v>
+      </c>
+      <c r="XZ1319" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>649,1318</v>
+      </c>
+      <c r="YA1319" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>650,1318</v>
+      </c>
+      <c r="YB1319" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>651,1318</v>
+      </c>
+    </row>
+    <row r="1320" spans="625:652" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XA1320" s="10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>624,1319</v>
+      </c>
+      <c r="XB1320" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>625,1319</v>
+      </c>
+      <c r="XC1320" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>626,1319</v>
+      </c>
+      <c r="XD1320" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>627,1319</v>
+      </c>
+      <c r="XE1320" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>628,1319</v>
+      </c>
+      <c r="XF1320" s="14" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>629,1319</v>
+      </c>
+      <c r="XL1320" s="11" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>635,1319</v>
+      </c>
+      <c r="XM1320" s="5" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>636,1319</v>
+      </c>
+      <c r="XN1320" s="15" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>637,1319</v>
+      </c>
+      <c r="XW1320" s="10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>646,1319</v>
+      </c>
+      <c r="XX1320" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>647,1319</v>
+      </c>
+      <c r="XY1320" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>648,1319</v>
+      </c>
+      <c r="XZ1320" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>649,1319</v>
+      </c>
+      <c r="YA1320" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>650,1319</v>
+      </c>
+      <c r="YB1320" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>651,1319</v>
+      </c>
+    </row>
+    <row r="1321" spans="625:652" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XA1321" s="11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>624,1320</v>
+      </c>
+      <c r="XB1321" s="13" t="str">
+        <f t="shared" ref="XA1321:XF1321" ca="1" si="9">CONCATENATE(CELL("col",XB1321)-1,",",CELL("row",XB1321)-1)</f>
+        <v>625,1320</v>
+      </c>
+      <c r="XC1321" s="13" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v>626,1320</v>
+      </c>
+      <c r="XD1321" s="13" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v>627,1320</v>
+      </c>
+      <c r="XE1321" s="13" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v>628,1320</v>
+      </c>
+      <c r="XF1321" s="15" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v>629,1320</v>
+      </c>
+      <c r="XG1321" s="7" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>630,1320</v>
+      </c>
+      <c r="XH1321" s="8" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>631,1320</v>
+      </c>
+      <c r="XI1321" s="8" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>632,1320</v>
+      </c>
+      <c r="XJ1321" s="8" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>633,1320</v>
+      </c>
+      <c r="XK1321" s="9" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>634,1320</v>
+      </c>
+      <c r="XL1321" s="7" t="str">
+        <f t="shared" ref="XL1321:XN1330" ca="1" si="10">CONCATENATE(CELL("col",XL1321)-1,",",CELL("row",XL1321)-1)</f>
+        <v>635,1320</v>
+      </c>
+      <c r="XM1321" s="16" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1320</v>
+      </c>
+      <c r="XN1321" s="9" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1320</v>
+      </c>
+      <c r="XW1321" s="11" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>646,1320</v>
+      </c>
+      <c r="XX1321" s="13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>647,1320</v>
+      </c>
+      <c r="XY1321" s="13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>648,1320</v>
+      </c>
+      <c r="XZ1321" s="13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>649,1320</v>
+      </c>
+      <c r="YA1321" s="13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>650,1320</v>
+      </c>
+      <c r="YB1321" s="15" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>651,1320</v>
+      </c>
+    </row>
+    <row r="1322" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XG1322" s="10" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>630,1321</v>
+      </c>
+      <c r="XH1322" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>631,1321</v>
+      </c>
+      <c r="XI1322" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>632,1321</v>
+      </c>
+      <c r="XJ1322" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>633,1321</v>
+      </c>
+      <c r="XK1322" s="14" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>634,1321</v>
+      </c>
+      <c r="XL1322" s="10" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1321</v>
+      </c>
+      <c r="XM1322" s="3" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1321</v>
+      </c>
+      <c r="XN1322" s="14" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1321</v>
+      </c>
+    </row>
+    <row r="1323" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XG1323" s="10" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>630,1322</v>
+      </c>
+      <c r="XH1323" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>631,1322</v>
+      </c>
+      <c r="XI1323" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>632,1322</v>
+      </c>
+      <c r="XJ1323" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="XK1323" s="4" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>634,1322</v>
+      </c>
+      <c r="XL1323" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1322</v>
+      </c>
+      <c r="XM1323" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="XN1323" s="14" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1322</v>
+      </c>
+    </row>
+    <row r="1324" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XG1324" s="10" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>630,1323</v>
+      </c>
+      <c r="XH1324" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>631,1323</v>
+      </c>
+      <c r="XI1324" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>632,1323</v>
+      </c>
+      <c r="XJ1324" s="3" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>633,1323</v>
+      </c>
+      <c r="XK1324" s="14" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>634,1323</v>
+      </c>
+      <c r="XL1324" s="10" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1323</v>
+      </c>
+      <c r="XM1324" s="3" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1323</v>
+      </c>
+      <c r="XN1324" s="14" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1323</v>
+      </c>
+    </row>
+    <row r="1325" spans="625:652" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XG1325" s="11" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>630,1324</v>
+      </c>
+      <c r="XH1325" s="13" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>631,1324</v>
+      </c>
+      <c r="XI1325" s="13" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>632,1324</v>
+      </c>
+      <c r="XJ1325" s="13" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>633,1324</v>
+      </c>
+      <c r="XK1325" s="15" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>634,1324</v>
+      </c>
+      <c r="XL1325" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1324</v>
+      </c>
+      <c r="XM1325" s="5" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1324</v>
+      </c>
+      <c r="XN1325" s="15" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1324</v>
+      </c>
+    </row>
+    <row r="1326" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XG1326" s="7" t="str">
+        <f t="shared" ref="XG1326:XK1330" ca="1" si="11">CONCATENATE(CELL("col",XG1326)-1,",",CELL("row",XG1326)-1)</f>
+        <v>630,1325</v>
+      </c>
+      <c r="XH1326" s="8" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>631,1325</v>
+      </c>
+      <c r="XI1326" s="8" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>632,1325</v>
+      </c>
+      <c r="XJ1326" s="8" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>633,1325</v>
+      </c>
+      <c r="XK1326" s="9" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>634,1325</v>
+      </c>
+      <c r="XL1326" s="7" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1325</v>
+      </c>
+      <c r="XM1326" s="16" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1325</v>
+      </c>
+      <c r="XN1326" s="9" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1325</v>
+      </c>
+    </row>
+    <row r="1327" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XG1327" s="10" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>630,1326</v>
+      </c>
+      <c r="XH1327" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>631,1326</v>
+      </c>
+      <c r="XI1327" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>632,1326</v>
+      </c>
+      <c r="XJ1327" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>633,1326</v>
+      </c>
+      <c r="XK1327" s="14" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>634,1326</v>
+      </c>
+      <c r="XL1327" s="10" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1326</v>
+      </c>
+      <c r="XM1327" s="3" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1326</v>
+      </c>
+      <c r="XN1327" s="14" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1326</v>
+      </c>
+    </row>
+    <row r="1328" spans="625:652" x14ac:dyDescent="0.3">
+      <c r="XG1328" s="10" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>630,1327</v>
+      </c>
+      <c r="XH1328" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>631,1327</v>
+      </c>
+      <c r="XI1328" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>632,1327</v>
+      </c>
+      <c r="XJ1328" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="XK1328" s="4" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>634,1327</v>
+      </c>
+      <c r="XL1328" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1327</v>
+      </c>
+      <c r="XM1328" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="XN1328" s="14" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1327</v>
+      </c>
+    </row>
+    <row r="1329" spans="631:656" x14ac:dyDescent="0.3">
+      <c r="XG1329" s="10" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>630,1328</v>
+      </c>
+      <c r="XH1329" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>631,1328</v>
+      </c>
+      <c r="XI1329" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>632,1328</v>
+      </c>
+      <c r="XJ1329" s="3" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>633,1328</v>
+      </c>
+      <c r="XK1329" s="14" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>634,1328</v>
+      </c>
+      <c r="XL1329" s="10" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1328</v>
+      </c>
+      <c r="XM1329" s="3" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1328</v>
+      </c>
+      <c r="XN1329" s="14" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1328</v>
+      </c>
+    </row>
+    <row r="1330" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XG1330" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>630,1329</v>
+      </c>
+      <c r="XH1330" s="13" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>631,1329</v>
+      </c>
+      <c r="XI1330" s="13" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>632,1329</v>
+      </c>
+      <c r="XJ1330" s="13" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>633,1329</v>
+      </c>
+      <c r="XK1330" s="15" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>634,1329</v>
+      </c>
+      <c r="XL1330" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>635,1329</v>
+      </c>
+      <c r="XM1330" s="5" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>636,1329</v>
+      </c>
+      <c r="XN1330" s="15" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>637,1329</v>
+      </c>
+    </row>
     <row r="1331" spans="631:656" x14ac:dyDescent="0.3">
       <c r="XG1331" s="7" t="str">
-        <f t="shared" ref="XG1331:YF1341" ca="1" si="0">CONCATENATE(CELL("col",XG1331)-1,",",CELL("row",XG1331)-1)</f>
+        <f t="shared" ref="XG1331:YF1341" ca="1" si="12">CONCATENATE(CELL("col",XG1331)-1,",",CELL("row",XG1331)-1)</f>
         <v>630,1330</v>
       </c>
       <c r="XH1331" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>631,1330</v>
       </c>
       <c r="XI1331" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>632,1330</v>
       </c>
       <c r="XJ1331" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>633,1330</v>
       </c>
       <c r="XK1331" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>634,1330</v>
       </c>
       <c r="XL1331" s="7" t="str">
-        <f t="shared" ref="XL1331:XL1332" ca="1" si="1">CONCATENATE(CELL("col",XL1331)-1,",",CELL("row",XL1331)-1)</f>
+        <f t="shared" ref="XL1331:XL1332" ca="1" si="13">CONCATENATE(CELL("col",XL1331)-1,",",CELL("row",XL1331)-1)</f>
         <v>635,1330</v>
       </c>
       <c r="XM1331" s="16" t="str">
-        <f t="shared" ref="XM1331:XN1331" ca="1" si="2">CONCATENATE(CELL("col",XM1331)-1,",",CELL("row",XM1331)-1)</f>
+        <f t="shared" ref="XM1331:XN1331" ca="1" si="14">CONCATENATE(CELL("col",XM1331)-1,",",CELL("row",XM1331)-1)</f>
         <v>636,1330</v>
       </c>
       <c r="XN1331" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="14"/>
         <v>637,1330</v>
       </c>
     </row>
     <row r="1332" spans="631:656" x14ac:dyDescent="0.3">
       <c r="XG1332" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>630,1331</v>
       </c>
       <c r="XH1332" s="3" t="str">
-        <f t="shared" ref="XH1332:XJ1334" ca="1" si="3">CONCATENATE(CELL("col",XH1332)-1,",",CELL("row",XH1332)-1)</f>
+        <f t="shared" ref="XH1332:XJ1334" ca="1" si="15">CONCATENATE(CELL("col",XH1332)-1,",",CELL("row",XH1332)-1)</f>
         <v>631,1331</v>
       </c>
       <c r="XI1332" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="15"/>
         <v>632,1331</v>
       </c>
       <c r="XJ1332" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="15"/>
         <v>633,1331</v>
       </c>
       <c r="XK1332" s="14" t="str">
-        <f t="shared" ref="XK1332:XN1334" ca="1" si="4">CONCATENATE(CELL("col",XK1332)-1,",",CELL("row",XK1332)-1)</f>
+        <f t="shared" ref="XK1332:XN1334" ca="1" si="16">CONCATENATE(CELL("col",XK1332)-1,",",CELL("row",XK1332)-1)</f>
         <v>634,1331</v>
       </c>
       <c r="XL1332" s="10" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="13"/>
         <v>635,1331</v>
       </c>
       <c r="XM1332" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="16"/>
         <v>636,1331</v>
       </c>
       <c r="XN1332" s="14" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="16"/>
         <v>637,1331</v>
       </c>
     </row>
     <row r="1333" spans="631:656" x14ac:dyDescent="0.3">
       <c r="XG1333" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>630,1332</v>
       </c>
       <c r="XH1333" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="15"/>
         <v>631,1332</v>
       </c>
       <c r="XI1333" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="15"/>
         <v>632,1332</v>
       </c>
       <c r="XJ1333" s="6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="XK1333" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>634,1332</v>
       </c>
       <c r="XL1333" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1332</v>
       </c>
       <c r="XM1333" s="6" t="s">
         <v>4</v>
       </c>
       <c r="XN1333" s="14" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="16"/>
         <v>637,1332</v>
       </c>
     </row>
     <row r="1334" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XG1334" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>630,1333</v>
       </c>
       <c r="XH1334" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="15"/>
         <v>631,1333</v>
       </c>
       <c r="XI1334" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="15"/>
         <v>632,1333</v>
       </c>
       <c r="XJ1334" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="15"/>
         <v>633,1333</v>
       </c>
       <c r="XK1334" s="14" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="16"/>
         <v>634,1333</v>
       </c>
       <c r="XL1334" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1333</v>
       </c>
       <c r="XM1334" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="16"/>
         <v>636,1333</v>
       </c>
       <c r="XN1334" s="14" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="16"/>
         <v>637,1333</v>
       </c>
     </row>
     <row r="1335" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XG1335" s="11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>630,1334</v>
       </c>
       <c r="XH1335" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>631,1334</v>
       </c>
       <c r="XI1335" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>632,1334</v>
       </c>
       <c r="XJ1335" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>633,1334</v>
       </c>
       <c r="XK1335" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>634,1334</v>
       </c>
       <c r="XL1335" s="11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1334</v>
       </c>
       <c r="XM1335" s="5" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>636,1334</v>
       </c>
       <c r="XN1335" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>637,1334</v>
       </c>
       <c r="XZ1335" s="7" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>649,1334</v>
       </c>
       <c r="YA1335" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>650,1334</v>
       </c>
       <c r="YB1335" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>651,1334</v>
       </c>
       <c r="YC1335" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>652,1334</v>
       </c>
       <c r="YD1335" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>653,1334</v>
       </c>
       <c r="YE1335" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>654,1334</v>
       </c>
       <c r="YF1335" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>655,1334</v>
       </c>
     </row>
     <row r="1336" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1336" s="7" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1335</v>
       </c>
       <c r="XM1336" s="16" t="str">
-        <f t="shared" ref="XM1336:XM1337" ca="1" si="5">CONCATENATE(CELL("col",XM1336)-1,",",CELL("row",XM1336)-1)</f>
+        <f t="shared" ref="XM1336:XM1337" ca="1" si="17">CONCATENATE(CELL("col",XM1336)-1,",",CELL("row",XM1336)-1)</f>
         <v>636,1335</v>
       </c>
       <c r="XN1336" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>637,1335</v>
       </c>
       <c r="XP1336" s="7" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>639,1335</v>
       </c>
       <c r="XQ1336" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>640,1335</v>
       </c>
       <c r="XR1336" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>641,1335</v>
       </c>
       <c r="XS1336" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>642,1335</v>
       </c>
       <c r="XT1336" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>643,1335</v>
       </c>
       <c r="XZ1336" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>649,1335</v>
       </c>
       <c r="YA1336" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>650,1335</v>
       </c>
       <c r="YB1336" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>651,1335</v>
       </c>
       <c r="YC1336" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>652,1335</v>
       </c>
       <c r="YD1336" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>653,1335</v>
       </c>
       <c r="YE1336" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>654,1335</v>
       </c>
       <c r="YF1336" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>655,1335</v>
       </c>
     </row>
     <row r="1337" spans="631:656" x14ac:dyDescent="0.3">
       <c r="XL1337" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1336</v>
       </c>
       <c r="XM1337" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="17"/>
         <v>636,1336</v>
       </c>
       <c r="XN1337" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>637,1336</v>
       </c>
       <c r="XO1337" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>638,1336</v>
       </c>
       <c r="XP1337" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>639,1336</v>
       </c>
       <c r="XQ1337" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>640,1336</v>
       </c>
       <c r="XR1337" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>641,1336</v>
       </c>
       <c r="XS1337" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>642,1336</v>
       </c>
       <c r="XT1337" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>643,1336</v>
       </c>
       <c r="XU1337" s="7" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>644,1336</v>
       </c>
       <c r="XV1337" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>645,1336</v>
       </c>
       <c r="XW1337" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>646,1336</v>
       </c>
       <c r="XX1337" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>647,1336</v>
       </c>
       <c r="XY1337" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>648,1336</v>
       </c>
       <c r="XZ1337" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>649,1336</v>
       </c>
       <c r="YA1337" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>650,1336</v>
       </c>
       <c r="YB1337" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>651,1336</v>
       </c>
       <c r="YC1337" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>652,1336</v>
       </c>
       <c r="YD1337" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>653,1336</v>
       </c>
       <c r="YE1337" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>654,1336</v>
       </c>
       <c r="YF1337" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>655,1336</v>
       </c>
     </row>
     <row r="1338" spans="631:656" x14ac:dyDescent="0.3">
       <c r="XL1338" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1337</v>
       </c>
       <c r="XM1338" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="XN1338" s="3" t="str">
-        <f t="shared" ref="XN1338:XN1339" ca="1" si="6">CONCATENATE(CELL("col",XN1338)-1,",",CELL("row",XN1338)-1)</f>
+        <f t="shared" ref="XN1338:XN1339" ca="1" si="18">CONCATENATE(CELL("col",XN1338)-1,",",CELL("row",XN1338)-1)</f>
         <v>637,1337</v>
       </c>
       <c r="XO1338" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>638,1337</v>
       </c>
       <c r="XP1338" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>639,1337</v>
       </c>
       <c r="XQ1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>640,1337</v>
       </c>
       <c r="XR1338" s="6" t="s">
         <v>0</v>
       </c>
       <c r="XS1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>642,1337</v>
       </c>
       <c r="XT1338" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>643,1337</v>
       </c>
       <c r="XU1338" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>644,1337</v>
       </c>
       <c r="XV1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>645,1337</v>
       </c>
       <c r="XW1338" s="6" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="XX1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>647,1337</v>
       </c>
       <c r="XY1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>648,1337</v>
       </c>
       <c r="XZ1338" s="2" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>649,1337</v>
       </c>
       <c r="YA1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>650,1337</v>
       </c>
       <c r="YB1338" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>651,1337</v>
       </c>
       <c r="YC1338" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="YD1338" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>653,1337</v>
       </c>
       <c r="YE1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>654,1337</v>
       </c>
       <c r="YF1338" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>655,1337</v>
       </c>
     </row>
     <row r="1339" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1339" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1338</v>
       </c>
       <c r="XM1339" s="3" t="str">
-        <f t="shared" ref="XM1339" ca="1" si="7">CONCATENATE(CELL("col",XM1339)-1,",",CELL("row",XM1339)-1)</f>
+        <f t="shared" ref="XM1339" ca="1" si="19">CONCATENATE(CELL("col",XM1339)-1,",",CELL("row",XM1339)-1)</f>
         <v>636,1338</v>
       </c>
       <c r="XN1339" s="3" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="18"/>
         <v>637,1338</v>
       </c>
       <c r="XO1339" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>638,1338</v>
       </c>
       <c r="XP1339" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>639,1338</v>
       </c>
       <c r="XQ1339" s="3" t="str">
-        <f t="shared" ref="XQ1339:XS1340" ca="1" si="8">CONCATENATE(CELL("col",XQ1339)-1,",",CELL("row",XQ1339)-1)</f>
+        <f t="shared" ref="XQ1339:XS1340" ca="1" si="20">CONCATENATE(CELL("col",XQ1339)-1,",",CELL("row",XQ1339)-1)</f>
         <v>640,1338</v>
       </c>
       <c r="XR1339" s="3" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="20"/>
         <v>641,1338</v>
       </c>
       <c r="XS1339" s="3" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="20"/>
         <v>642,1338</v>
       </c>
       <c r="XT1339" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>643,1338</v>
       </c>
       <c r="XU1339" s="11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>644,1338</v>
       </c>
       <c r="XV1339" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>645,1338</v>
       </c>
       <c r="XW1339" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>646,1338</v>
       </c>
       <c r="XX1339" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>647,1338</v>
       </c>
       <c r="XY1339" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>648,1338</v>
       </c>
       <c r="XZ1339" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>649,1338</v>
       </c>
       <c r="YA1339" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>650,1338</v>
       </c>
       <c r="YB1339" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>651,1338</v>
       </c>
       <c r="YC1339" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>652,1338</v>
       </c>
       <c r="YD1339" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>653,1338</v>
       </c>
       <c r="YE1339" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>654,1338</v>
       </c>
       <c r="YF1339" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>655,1338</v>
       </c>
     </row>
     <row r="1340" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1340" s="11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>635,1339</v>
       </c>
       <c r="XM1340" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>636,1339</v>
       </c>
       <c r="XN1340" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>637,1339</v>
       </c>
       <c r="XO1340" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>638,1339</v>
       </c>
       <c r="XP1340" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>639,1339</v>
       </c>
       <c r="XQ1340" s="12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>640,1339</v>
       </c>
       <c r="XR1340" s="3" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="20"/>
         <v>641,1339</v>
       </c>
       <c r="XS1340" s="12" t="str">
-        <f t="shared" ref="XS1340:XS1341" ca="1" si="9">CONCATENATE(CELL("col",XS1340)-1,",",CELL("row",XS1340)-1)</f>
+        <f t="shared" ref="XS1340:XS1341" ca="1" si="21">CONCATENATE(CELL("col",XS1340)-1,",",CELL("row",XS1340)-1)</f>
         <v>642,1339</v>
       </c>
       <c r="XT1340" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>643,1339</v>
       </c>
       <c r="XZ1340" s="10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>649,1339</v>
       </c>
       <c r="YA1340" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>650,1339</v>
       </c>
       <c r="YB1340" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>651,1339</v>
       </c>
       <c r="YC1340" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>652,1339</v>
       </c>
       <c r="YD1340" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>653,1339</v>
       </c>
       <c r="YE1340" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>654,1339</v>
       </c>
       <c r="YF1340" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>655,1339</v>
       </c>
     </row>
     <row r="1341" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XP1341" s="11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>639,1340</v>
       </c>
       <c r="XQ1341" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>640,1340</v>
       </c>
       <c r="XR1341" s="5" t="str">
-        <f t="shared" ref="XR1341" ca="1" si="10">CONCATENATE(CELL("col",XR1341)-1,",",CELL("row",XR1341)-1)</f>
+        <f t="shared" ref="XR1341" ca="1" si="22">CONCATENATE(CELL("col",XR1341)-1,",",CELL("row",XR1341)-1)</f>
         <v>641,1340</v>
       </c>
       <c r="XS1341" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="21"/>
         <v>642,1340</v>
       </c>
       <c r="XT1341" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>643,1340</v>
       </c>
       <c r="XZ1341" s="11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>649,1340</v>
       </c>
       <c r="YA1341" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>650,1340</v>
       </c>
       <c r="YB1341" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>651,1340</v>
       </c>
       <c r="YC1341" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>652,1340</v>
       </c>
       <c r="YD1341" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>653,1340</v>
       </c>
       <c r="YE1341" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>654,1340</v>
       </c>
       <c r="YF1341" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v>655,1340</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Thu Oct 11 21:24:59 EDT 2018
</commit_message>
<xml_diff>
--- a/WoFM RPG/Assets/JS/map.xlsx
+++ b/WoFM RPG/Assets/JS/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\588648\Unity\WoFM RPG\Assets\JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FD19AB62-1213-4801-B5F1-B3B503587E66}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FDE902FD-4D44-4D9D-9BA4-AF7B0F7346B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="XA1306:YF1341"/>
+  <dimension ref="XA1306:YB1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="XG1328" workbookViewId="0">
-      <selection activeCell="XU1310" sqref="XU1310"/>
+    <sheetView tabSelected="1" topLeftCell="XM1328" workbookViewId="0">
+      <selection activeCell="XY1346" sqref="XY1346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,7 +812,7 @@
         <v>624,1314</v>
       </c>
       <c r="XB1315" s="8" t="str">
-        <f t="shared" ref="XA1315:XF1320" ca="1" si="3">CONCATENATE(CELL("col",XB1315)-1,",",CELL("row",XB1315)-1)</f>
+        <f t="shared" ref="XB1315:XF1320" ca="1" si="3">CONCATENATE(CELL("col",XB1315)-1,",",CELL("row",XB1315)-1)</f>
         <v>625,1314</v>
       </c>
       <c r="XC1315" s="8" t="str">
@@ -1008,7 +1008,7 @@
         <v>634,1316</v>
       </c>
       <c r="XL1317" s="7" t="str">
-        <f t="shared" ref="XL1316:XW1319" ca="1" si="6">CONCATENATE(CELL("col",XL1317)-1,",",CELL("row",XL1317)-1)</f>
+        <f t="shared" ref="XL1317:XW1319" ca="1" si="6">CONCATENATE(CELL("col",XL1317)-1,",",CELL("row",XL1317)-1)</f>
         <v>635,1316</v>
       </c>
       <c r="XM1317" s="8" t="str">
@@ -1120,7 +1120,7 @@
         <v>634,1317</v>
       </c>
       <c r="XL1318" s="2" t="str">
-        <f t="shared" ref="XL1316:XS1320" ca="1" si="7">CONCATENATE(CELL("col",XL1318)-1,",",CELL("row",XL1318)-1)</f>
+        <f t="shared" ref="XL1318:XN1320" ca="1" si="7">CONCATENATE(CELL("col",XL1318)-1,",",CELL("row",XL1318)-1)</f>
         <v>635,1317</v>
       </c>
       <c r="XM1318" s="6" t="s">
@@ -1366,7 +1366,7 @@
         <v>624,1320</v>
       </c>
       <c r="XB1321" s="13" t="str">
-        <f t="shared" ref="XA1321:XF1321" ca="1" si="9">CONCATENATE(CELL("col",XB1321)-1,",",CELL("row",XB1321)-1)</f>
+        <f t="shared" ref="XB1321:XF1321" ca="1" si="9">CONCATENATE(CELL("col",XB1321)-1,",",CELL("row",XB1321)-1)</f>
         <v>625,1320</v>
       </c>
       <c r="XC1321" s="13" t="str">
@@ -1676,7 +1676,7 @@
         <v>637,1327</v>
       </c>
     </row>
-    <row r="1329" spans="631:656" x14ac:dyDescent="0.3">
+    <row r="1329" spans="631:651" x14ac:dyDescent="0.3">
       <c r="XG1329" s="10" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>630,1328</v>
@@ -1710,7 +1710,7 @@
         <v>637,1328</v>
       </c>
     </row>
-    <row r="1330" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1330" spans="631:651" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XG1330" s="11" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>630,1329</v>
@@ -1744,9 +1744,9 @@
         <v>637,1329</v>
       </c>
     </row>
-    <row r="1331" spans="631:656" x14ac:dyDescent="0.3">
+    <row r="1331" spans="631:651" x14ac:dyDescent="0.3">
       <c r="XG1331" s="7" t="str">
-        <f t="shared" ref="XG1331:YF1341" ca="1" si="12">CONCATENATE(CELL("col",XG1331)-1,",",CELL("row",XG1331)-1)</f>
+        <f t="shared" ref="XG1331:YA1341" ca="1" si="12">CONCATENATE(CELL("col",XG1331)-1,",",CELL("row",XG1331)-1)</f>
         <v>630,1330</v>
       </c>
       <c r="XH1331" s="8" t="str">
@@ -1778,7 +1778,7 @@
         <v>637,1330</v>
       </c>
     </row>
-    <row r="1332" spans="631:656" x14ac:dyDescent="0.3">
+    <row r="1332" spans="631:651" x14ac:dyDescent="0.3">
       <c r="XG1332" s="10" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>630,1331</v>
@@ -1812,7 +1812,7 @@
         <v>637,1331</v>
       </c>
     </row>
-    <row r="1333" spans="631:656" x14ac:dyDescent="0.3">
+    <row r="1333" spans="631:651" x14ac:dyDescent="0.3">
       <c r="XG1333" s="10" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>630,1332</v>
@@ -1844,7 +1844,7 @@
         <v>637,1332</v>
       </c>
     </row>
-    <row r="1334" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1334" spans="631:651" x14ac:dyDescent="0.3">
       <c r="XG1334" s="10" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>630,1333</v>
@@ -1878,7 +1878,7 @@
         <v>637,1333</v>
       </c>
     </row>
-    <row r="1335" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1335" spans="631:651" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XG1335" s="11" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>630,1334</v>
@@ -1911,36 +1911,8 @@
         <f t="shared" ca="1" si="12"/>
         <v>637,1334</v>
       </c>
-      <c r="XZ1335" s="7" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>649,1334</v>
-      </c>
-      <c r="YA1335" s="8" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>650,1334</v>
-      </c>
-      <c r="YB1335" s="8" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>651,1334</v>
-      </c>
-      <c r="YC1335" s="8" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>652,1334</v>
-      </c>
-      <c r="YD1335" s="8" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>653,1334</v>
-      </c>
-      <c r="YE1335" s="8" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>654,1334</v>
-      </c>
-      <c r="YF1335" s="9" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>655,1334</v>
-      </c>
-    </row>
-    <row r="1336" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="1336" spans="631:651" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1336" s="7" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>635,1335</v>
@@ -1973,36 +1945,8 @@
         <f t="shared" ca="1" si="12"/>
         <v>643,1335</v>
       </c>
-      <c r="XZ1336" s="10" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>649,1335</v>
-      </c>
-      <c r="YA1336" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>650,1335</v>
-      </c>
-      <c r="YB1336" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>651,1335</v>
-      </c>
-      <c r="YC1336" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>652,1335</v>
-      </c>
-      <c r="YD1336" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>653,1335</v>
-      </c>
-      <c r="YE1336" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>654,1335</v>
-      </c>
-      <c r="YF1336" s="14" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>655,1335</v>
-      </c>
-    </row>
-    <row r="1337" spans="631:656" x14ac:dyDescent="0.3">
+    </row>
+    <row r="1337" spans="631:651" x14ac:dyDescent="0.3">
       <c r="XL1337" s="10" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>635,1336</v>
@@ -2059,36 +2003,16 @@
         <f t="shared" ca="1" si="12"/>
         <v>648,1336</v>
       </c>
-      <c r="XZ1337" s="10" t="str">
+      <c r="XZ1337" s="7" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>649,1336</v>
       </c>
-      <c r="YA1337" s="3" t="str">
+      <c r="YA1337" s="9" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>650,1336</v>
       </c>
-      <c r="YB1337" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>651,1336</v>
-      </c>
-      <c r="YC1337" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>652,1336</v>
-      </c>
-      <c r="YD1337" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>653,1336</v>
-      </c>
-      <c r="YE1337" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>654,1336</v>
-      </c>
-      <c r="YF1337" s="14" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>655,1336</v>
-      </c>
-    </row>
-    <row r="1338" spans="631:656" x14ac:dyDescent="0.3">
+    </row>
+    <row r="1338" spans="631:651" x14ac:dyDescent="0.3">
       <c r="XL1338" s="10" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>635,1337</v>
@@ -2142,35 +2066,15 @@
         <f t="shared" ca="1" si="12"/>
         <v>648,1337</v>
       </c>
-      <c r="XZ1338" s="2" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>649,1337</v>
-      </c>
-      <c r="YA1338" s="3" t="str">
+      <c r="XZ1338" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="YA1338" s="14" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>650,1337</v>
       </c>
-      <c r="YB1338" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>651,1337</v>
-      </c>
-      <c r="YC1338" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="YD1338" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>653,1337</v>
-      </c>
-      <c r="YE1338" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>654,1337</v>
-      </c>
-      <c r="YF1338" s="14" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>655,1337</v>
-      </c>
-    </row>
-    <row r="1339" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="1339" spans="631:651" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1339" s="10" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>635,1338</v>
@@ -2227,36 +2131,16 @@
         <f t="shared" ca="1" si="12"/>
         <v>648,1338</v>
       </c>
-      <c r="XZ1339" s="10" t="str">
+      <c r="XZ1339" s="11" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>649,1338</v>
       </c>
-      <c r="YA1339" s="3" t="str">
+      <c r="YA1339" s="15" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>650,1338</v>
       </c>
-      <c r="YB1339" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>651,1338</v>
-      </c>
-      <c r="YC1339" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>652,1338</v>
-      </c>
-      <c r="YD1339" s="12" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>653,1338</v>
-      </c>
-      <c r="YE1339" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>654,1338</v>
-      </c>
-      <c r="YF1339" s="14" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>655,1338</v>
-      </c>
-    </row>
-    <row r="1340" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="1340" spans="631:651" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1340" s="11" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>635,1339</v>
@@ -2293,36 +2177,8 @@
         <f t="shared" ca="1" si="12"/>
         <v>643,1339</v>
       </c>
-      <c r="XZ1340" s="10" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>649,1339</v>
-      </c>
-      <c r="YA1340" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>650,1339</v>
-      </c>
-      <c r="YB1340" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>651,1339</v>
-      </c>
-      <c r="YC1340" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>652,1339</v>
-      </c>
-      <c r="YD1340" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>653,1339</v>
-      </c>
-      <c r="YE1340" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>654,1339</v>
-      </c>
-      <c r="YF1340" s="14" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>655,1339</v>
-      </c>
-    </row>
-    <row r="1341" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="1341" spans="631:651" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XP1341" s="11" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>639,1340</v>
@@ -2342,34 +2198,6 @@
       <c r="XT1341" s="15" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>643,1340</v>
-      </c>
-      <c r="XZ1341" s="11" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>649,1340</v>
-      </c>
-      <c r="YA1341" s="13" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>650,1340</v>
-      </c>
-      <c r="YB1341" s="13" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>651,1340</v>
-      </c>
-      <c r="YC1341" s="13" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>652,1340</v>
-      </c>
-      <c r="YD1341" s="13" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>653,1340</v>
-      </c>
-      <c r="YE1341" s="13" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>654,1340</v>
-      </c>
-      <c r="YF1341" s="15" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>655,1340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sun Nov 18 20:58:43 EST 2018
</commit_message>
<xml_diff>
--- a/WoFM RPG/Assets/JS/map.xlsx
+++ b/WoFM RPG/Assets/JS/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\588648\Unity\WoFM RPG\Assets\JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FDE902FD-4D44-4D9D-9BA4-AF7B0F7346B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{68A01F8E-9F48-4FCF-924D-DD73C08DBDD6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="XA1306:YB1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="XM1328" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="XD1328" workbookViewId="0">
       <selection activeCell="XY1346" sqref="XY1346"/>
     </sheetView>
   </sheetViews>

</xml_diff>